<commit_message>
updated Operators Test case
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\BDDCucumber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF9436C-AA4A-4F3F-BE68-B1B4BF0DDBF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BFADB4-43A4-46EC-ACD5-4E41AB972370}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="4764" windowWidth="17280" windowHeight="7008" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="user" sheetId="3" r:id="rId3"/>
     <sheet name="register" sheetId="4" r:id="rId4"/>
     <sheet name="operator" sheetId="5" r:id="rId5"/>
-    <sheet name="usefullink" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="usefullink" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
   <si>
     <t>Username</t>
   </si>
@@ -194,9 +195,6 @@
     <t>Neelam</t>
   </si>
   <si>
-    <t>Technical Discussion(Errors, Software, Technical Materials)</t>
-  </si>
-  <si>
     <t>Whats App  Phone Call SMS eMail</t>
   </si>
   <si>
@@ -265,12 +263,92 @@
   <si>
     <t>Placement</t>
   </si>
+  <si>
+    <t>Technical Discussion (Errors, Software, Technical Materials)</t>
+  </si>
+  <si>
+    <r>
+      <t>Whats App</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Phone Call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SMS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>eMail</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>09:00 AM to 06:00 PM </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Monday to Friday and Sunday</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +375,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="6"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +417,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -386,6 +489,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,7 +1233,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,7 +1254,7 @@
         <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>39</v>
@@ -1172,10 +1291,10 @@
         <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="5">
         <v>7066885937</v>
@@ -1189,13 +1308,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5">
         <v>8888558802</v>
@@ -1209,19 +1328,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="6">
         <v>8888809416</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1229,10 +1348,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>42</v>
@@ -1241,7 +1360,7 @@
         <v>8866888662</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1251,10 +1370,150 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DD7FB3-F5D4-4F20-93A9-8501ADC161DA}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="52.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="12">
+        <v>9552343698</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="12">
+        <v>7066885937</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="12">
+        <v>8888558802</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="12">
+        <v>8888809416</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="14">
+        <v>8866888662</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61511D16-5CEE-4ECE-80C7-1A433DA9A101}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1265,13 +1524,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1279,10 +1538,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1290,10 +1549,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1301,10 +1560,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1312,10 +1571,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1326,7 +1585,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1334,10 +1593,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Excel for operator testcase
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\BDDCucumber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BFADB4-43A4-46EC-ACD5-4E41AB972370}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E0A389-AB23-4EED-B677-B48BB7F35265}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="user" sheetId="3" r:id="rId3"/>
     <sheet name="register" sheetId="4" r:id="rId4"/>
     <sheet name="operator" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="operator1" sheetId="7" r:id="rId6"/>
     <sheet name="usefullink" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -249,9 +249,6 @@
     <t>Schedule</t>
   </si>
   <si>
-    <t>Go!</t>
-  </si>
-  <si>
     <t>Video Lactures All Topics</t>
   </si>
   <si>
@@ -265,68 +262,6 @@
   </si>
   <si>
     <t>Technical Discussion (Errors, Software, Technical Materials)</t>
-  </si>
-  <si>
-    <r>
-      <t>Whats App</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Phone Call</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="6"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>eMail</t>
-    </r>
   </si>
   <si>
     <r>
@@ -343,12 +278,18 @@
       <t>Monday to Friday and Sunday</t>
     </r>
   </si>
+  <si>
+    <t>Whats App Phone Call SMS eMail</t>
+  </si>
+  <si>
+    <t>Go !</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,15 +322,8 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <b/>
-      <sz val="6"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,18 +351,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -490,21 +412,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1291,7 +1206,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>46</v>
@@ -1374,37 +1289,38 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="52.88671875" customWidth="1"/>
     <col min="4" max="4" width="26.21875" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1414,7 +1330,7 @@
       <c r="C2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="12">
@@ -1424,7 +1340,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1432,7 +1348,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>66</v>
@@ -1444,7 +1360,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1464,7 +1380,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1481,31 +1397,32 @@
         <v>8888809416</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>8866888662</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1514,7 +1431,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,7 +1458,7 @@
         <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1549,10 +1466,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1560,10 +1477,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1571,10 +1488,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1585,7 +1502,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1593,10 +1510,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>